<commit_message>
Remove hist and final excel upda
</commit_message>
<xml_diff>
--- a/Chap Preferences.xlsx
+++ b/Chap Preferences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frederickpickering/gitRepos/ChaPerrone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38387CDC-9804-0B43-9783-7ABC7C0827C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235BA30B-A1BE-A34E-AEAF-7D9CE767349C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Choices" sheetId="1" r:id="rId1"/>
@@ -1268,7 +1268,7 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -4542,8 +4542,8 @@
   </sheetPr>
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>